<commit_message>
Fix: change application architecture
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t xml:space="preserve">SurveyService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Реконструкция архитектуры Polygon, Catalog domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polygon*, Catalog*</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -539,10 +545,10 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -607,10 +613,18 @@
       <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>45632</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.118055555555556</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,12 +706,12 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="n">
         <f aca="false">SUM(C3:C16)</f>
-        <v>0.215277777777778</v>
+        <v>0.333333333333334</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="11"/>
@@ -736,7 +750,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -762,96 +776,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="X1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="Z1" s="19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AA1" s="19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AB1" s="19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="20" t="n">
         <v>100000</v>
@@ -942,7 +956,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="20" t="n">
         <v>100000</v>
@@ -1033,7 +1047,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="20" t="n">
         <v>100000</v>
@@ -1124,7 +1138,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="20" t="n">
         <v>-100000</v>
@@ -1716,13 +1730,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,7 +1840,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -1840,37 +1854,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Feat: layer isolation has finished
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">PolygonService, CatalogService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taheoport.*</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -575,10 +578,10 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -763,10 +766,18 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>45644</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>0.111111111111111</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,12 +803,12 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="n">
         <f aca="false">SUM(C3:C16)</f>
-        <v>1.19791666666667</v>
+        <v>1.30902777777778</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="11"/>
@@ -836,7 +847,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -862,96 +873,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="J1" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="18" t="s">
-        <v>33</v>
-      </c>
       <c r="R1" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="18" t="s">
-        <v>38</v>
-      </c>
       <c r="X1" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Y1" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA1" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB1" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="20" t="n">
         <v>100000</v>
@@ -1042,7 +1053,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="20" t="n">
         <v>100000</v>
@@ -1133,7 +1144,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="20" t="n">
         <v>100000</v>
@@ -1224,7 +1235,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" s="20" t="n">
         <v>-100000</v>
@@ -1816,13 +1827,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1937,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -1940,37 +1951,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: injection to project the DependencyInjector
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t xml:space="preserve">DataHandlerTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Внедрение интерфейса DependencyInjector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DependencyInjector</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -587,13 +593,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -823,32 +829,61 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>45649</v>
+      </c>
+      <c r="C16" s="7" t="n">
+        <v>0.260416666666667</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13" t="n">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13" t="n">
         <f aca="false">SUM(C3:C16)</f>
-        <v>1.43055555555556</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="15"/>
+        <v>1.69097222222222</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -875,7 +910,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -901,96 +936,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>30</v>
-      </c>
       <c r="J1" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="X1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="Z1" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AA1" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AB1" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B2" s="20" t="n">
         <v>100000</v>
@@ -1081,7 +1116,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" s="20" t="n">
         <v>100000</v>
@@ -1172,7 +1207,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" s="20" t="n">
         <v>100000</v>
@@ -1263,7 +1298,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="20" t="n">
         <v>-100000</v>
@@ -1855,13 +1890,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,7 +2000,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -1979,37 +2014,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Work: Injection to project the class DependencyContainer
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">DependencyInjector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Внедрение класса DependencyContainer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DependencyContainer</t>
   </si>
   <si>
     <t xml:space="preserve">Сумма</t>
@@ -596,10 +602,10 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -844,10 +850,18 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>45649</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <v>0.0243055555555556</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +880,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="13" t="n">
@@ -910,7 +924,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -936,96 +950,96 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" s="17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="X1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="18" t="s">
-        <v>45</v>
-      </c>
       <c r="Z1" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AA1" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB1" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2" s="20" t="n">
         <v>100000</v>
@@ -1116,7 +1130,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" s="20" t="n">
         <v>100000</v>
@@ -1207,7 +1221,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B4" s="20" t="n">
         <v>100000</v>
@@ -1298,7 +1312,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B5" s="20" t="n">
         <v>-100000</v>
@@ -1890,13 +1904,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,7 +2014,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -2014,37 +2028,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Feat: DependencyContainer and DependencyInjector has bin injecting
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -605,7 +605,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -865,10 +865,18 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
+      <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>45651</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>0.0555555555555556</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +932,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -2014,7 +2022,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>

</xml_diff>

<commit_message>
Work: developing tests for GeoCalculator
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -608,10 +608,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -901,10 +901,18 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>45652</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +982,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -2064,7 +2072,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>

</xml_diff>

<commit_message>
Feat: tests developing for GeoCalculator
</commit_message>
<xml_diff>
--- a/project_journal.xlsx
+++ b/project_journal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t xml:space="preserve">Краткое описание выполненной работы</t>
   </si>
@@ -608,10 +608,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.86"/>
@@ -916,10 +916,18 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>45653</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>0.0347222222222222</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +990,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
@@ -2072,7 +2080,7 @@
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>

</xml_diff>